<commit_message>
Added features - Apache POI, Broken Links, Test Automation Framework, Data driven Framework, Log 4j ------ ALL Combined
</commit_message>
<xml_diff>
--- a/Selenium-Tips.xlsx
+++ b/Selenium-Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\eclipse-workspace\SeleniumMaven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC003F8-2CD1-4872-B3FB-A6FF7F4A28D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A9CBE1-E499-4B39-AD3C-17E3AC069935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1800" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ACE05C23-1BF1-42A7-90BC-827259F13849}"/>
+    <workbookView xWindow="28680" yWindow="-1800" windowWidth="29040" windowHeight="15840" xr2:uid="{ACE05C23-1BF1-42A7-90BC-827259F13849}"/>
   </bookViews>
   <sheets>
     <sheet name="Selenium Tips" sheetId="1" r:id="rId1"/>
@@ -502,10 +502,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4F9A38-D0A6-47F1-9877-24377C89BC1E}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,10 +997,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1160,12 +1160,12 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1195,27 +1195,32 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B47" s="3"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B48" s="1" t="s">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="1" t="s">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="1" t="s">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
+      <c r="A51" s="3"/>
+      <c r="B51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1235,7 +1240,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1252,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4843D49-18D8-4E17-912A-E6CA89D8AF31}">
   <dimension ref="A52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -1530,7 +1535,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>